<commit_message>
1.增加:sdio spi uart 底层设置;
</commit_message>
<xml_diff>
--- a/3.引脚资源配置/引脚资源配置.xlsx
+++ b/3.引脚资源配置/引脚资源配置.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>SPI1_NSS</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -66,107 +66,145 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>LCD_RST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD_A0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SPI2_SCK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SPI2_MOSI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上拉开背景灯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上拉供电</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上拉让BLE通电</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PD0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PD2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PD1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PD4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PD3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SPI2_MISO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>晶振</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OSC_IN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OSC_OUT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PF0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PF1</t>
+  </si>
+  <si>
+    <t>OSC32_IN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OSC32_OUT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC15</t>
+  </si>
+  <si>
+    <t>外部大晶振</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>LCD_CS</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>LCD_RST</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LCD_A0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SPI2_SCK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SPI2_MOSI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>LCD_BK</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>CTL_LCD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>上拉开背景灯</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>上拉供电</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PA4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PA7</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PA1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PA6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PA9</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>上拉让BLE通电</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PC5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PC4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PC7</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PC9</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PD0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PD2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PD1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PD4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PD3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SPI2_MISO</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PC6</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -190,7 +228,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,6 +253,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -228,11 +272,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -534,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -556,7 +601,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
@@ -564,7 +609,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
@@ -572,7 +617,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
@@ -580,7 +625,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
@@ -588,7 +633,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>5</v>
@@ -602,7 +647,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.15">
@@ -610,7 +655,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.15">
@@ -618,10 +663,10 @@
         <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.15">
@@ -629,77 +674,116 @@
         <v>11</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B10" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B11" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B12" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B13" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B15" s="3" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B16" s="3" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B18" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>20</v>
+      <c r="C18" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B20" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>